<commit_message>
added new changes to excel file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="13">
   <si>
     <t>dwa</t>
   </si>
@@ -378,7 +378,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,7 +460,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -494,7 +494,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -527,6 +527,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
@@ -535,6 +538,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
@@ -546,6 +552,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -564,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>

</xml_diff>